<commit_message>
commit before 1st class
</commit_message>
<xml_diff>
--- a/material/data/schedule.xlsx
+++ b/material/data/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebstier/Library/CloudStorage/Dropbox/Lehrveranstaltungen/2024 - Mannheim/ma_css24/material/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebstier/Library/CloudStorage/Dropbox/Lehrveranstaltungen/2024-25 - Mannheim/ma_css24-25/material/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458C1EBC-4E5E-8F4B-822D-57C656B548C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45DCFCF-B90D-524C-BCC6-501840C9D9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{6C7A0B95-C424-6845-B994-5F3721DB8565}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{6C7A0B95-C424-6845-B994-5F3721DB8565}"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -25,116 +25,152 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>14 February 2024</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>22 May 2024</t>
-  </si>
-  <si>
-    <t>17 April 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 March 2024 </t>
-  </si>
-  <si>
     <t>Required reading</t>
   </si>
   <si>
-    <t>- Introduction
-- Foundations of CSS
-- The tidyverse
+    <t>Topics</t>
+  </si>
+  <si>
+    <t>Lazer, D., &amp; Radford, J. (2017). Data ex Machina: Introduction to Big Data. [*Annual Review of Sociology*, 43(1), 19–39.](https://doi.org/10.1146/annurev-soc-060116-053457)</t>
+  </si>
+  <si>
+    <t>Bauer, P. C., &amp; Landesvatter, C. (2023). Writing a reproducible paper with RStudio and Quarto. [*OSF Preprint*.](https://doi.org/10.31219/osf.io/ur4xn)</t>
+  </si>
+  <si>
+    <t>Gilardi, F., Alizadeh, M., &amp; Kubli, M. (2023). ChatGPT outperforms crowd workers for text-annotation tasks. [*PNAS*, 120(30).](https://doi.org/10.1073/pnas.2305016120)  &lt;br/&gt;&lt;br/&gt;
+Reiss, M. V. (2023). Testing the Reliability of ChatGPT for Text Annotation and Classification: A Cautionary Remark. [*arXiv Preprint*.](http://arxiv.org/abs/2304.11085)</t>
+  </si>
+  <si>
+    <t>Fiesler, C., &amp; Proferes, N. (2018). 'Participant' Perceptions of Twitter Research Ethics. [*Social Media + Society*, 4(1).](https://doi.org/10.1177/2056305118763366) &lt;br/&gt;&lt;br/&gt;
+Freelon, D. (2018). Computational Research in the Post-API Age. [*Political Communication*, 35(4), 665–668.](https://osf.io/preprints/socarxiv/56f4q)</t>
+  </si>
+  <si>
+    <t>- Presentations of thesis ideas
+- Coding: troubleshooting</t>
+  </si>
+  <si>
+    <t>3 September 2024</t>
+  </si>
+  <si>
+    <t>11 September 2024</t>
+  </si>
+  <si>
+    <t>2 October 2024</t>
+  </si>
+  <si>
+    <t>9 October 2024</t>
+  </si>
+  <si>
+    <t>16 October 2024</t>
+  </si>
+  <si>
+    <t>23 October 2024</t>
+  </si>
+  <si>
+    <t>30 October 2024</t>
+  </si>
+  <si>
+    <t>6 November 2024</t>
+  </si>
+  <si>
+    <t>13 November 2024</t>
+  </si>
+  <si>
+    <t>20 November 2024</t>
+  </si>
+  <si>
+    <t>27 November 2024</t>
+  </si>
+  <si>
+    <t>4 December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Machine learning
+- Large Language Models </t>
+  </si>
+  <si>
+    <t>- Open science and reproducibility in CSS</t>
+  </si>
+  <si>
+    <t>- Data quality and validation in CSS
+- Network analysis</t>
+  </si>
+  <si>
+    <t>- Writing reproducible research papers in R
+- R Markdown, quarto</t>
+  </si>
+  <si>
+    <t>- Foundations of CSS
+- The R tidyverse</t>
+  </si>
+  <si>
+    <t>- Social media, web data and web scraping
+- APIs and web data collection</t>
+  </si>
+  <si>
+    <t>- Research ethics in CSS 
 - Data visualization</t>
   </si>
   <si>
-    <t>- Research ethics in CSS 
-- Social media and web data 
-- APIs
-- Web scraping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Designed digital data 
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Chan, C.- Hong, Schatto-Eckrodt, T., &amp; Gruber, J. (2024). What makes computational communication science (ir)reproducible? [*Computational Communication Research*, 6(1).](https://doi.org/10.5117/CCR2024.1.5.CHAN) &lt;br/&gt;&lt;br/&gt;
+Nyhan, B., Settle, J., Thorson, E., Wojcieszak, M., Barberá, P., et al. (2023). Like-minded sources on Facebook are prevalent but not polarizing. [*Nature*, 620(7972), 137–144.](https://doi.org/10.1038/s41586-023-06297-w)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Linked surveys and DBD 
 - Web tracking data 
 - Smartphone-based data collection 
-- Linked surveys and DBD </t>
-  </si>
-  <si>
-    <t>Topics</t>
-  </si>
-  <si>
-    <t>Lazer, D., &amp; Radford, J. (2017). Data ex Machina: Introduction to Big Data. [*Annual Review of Sociology*, 43(1), 19–39.](https://doi.org/10.1146/annurev-soc-060116-053457)</t>
-  </si>
-  <si>
-    <t>- Presentations of thesis ideas 
-- Coding: troubleshooting</t>
-  </si>
-  <si>
-    <t>Bauer, P. C., &amp; Landesvatter, C. (2023). Writing a reproducible paper with RStudio and Quarto. [*OSF Preprint*.](https://doi.org/10.31219/osf.io/ur4xn)</t>
-  </si>
-  <si>
-    <t>Gilardi, F., Alizadeh, M., &amp; Kubli, M. (2023). ChatGPT outperforms crowd workers for text-annotation tasks. [*PNAS*, 120(30).](https://doi.org/10.1073/pnas.2305016120)  &lt;br/&gt;&lt;br/&gt;
-Reiss, M. V. (2023). Testing the Reliability of ChatGPT for Text Annotation and Classification: A Cautionary Remark. [*arXiv Preprint*.](http://arxiv.org/abs/2304.11085)</t>
+</t>
+  </si>
+  <si>
+    <t>- Introduction to automated text analysis
+- Supervised and unsupervised models
+- Validation of model results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schwemmer, C., &amp; Wieczorek, O. (2020). The Methodological Divide of Sociology: Evidence from Two Decades of Journal Publications. [*Sociology*, 54(1), 3–21.](https://doi.org/10.1177/0038038519853146) &lt;br/&gt;&lt;br/&gt;
+Bonikowski, B., Luo, Y., &amp; Stuhler, O. (2022). Politics as Usual? Measuring Populism, Nationalism, and Authoritarianism in U.S. Presidential Campaigns (1952–2020) with Neural Language Models. [*Sociological Methods &amp; Research*, 51(4), 1721–1787.](https://doi.org/10.31235/osf.io/uhvbp) </t>
+  </si>
+  <si>
+    <t>- Introduction and expectations
+- Foundations of CSS
+- Getting started in R</t>
+  </si>
+  <si>
+    <t>Sen, I., Flöck, F., Weller, K., Weiß, B., &amp; Wagner, C. (2021). A Total Error Framework for Digital Traces of Human Behavior on Online Platforms. [*Public Opinion Quarterly*, 85(S1), 399–422.](https://doi.org/10.1093/poq/nfab018) &lt;br/&gt;&lt;br/&gt;
+Dahlke, R., Kumar, D., Durumeric, Z., &amp; Hancock, J. T. (2023). Quantifying the Systematic Bias in the Accessibility and Inaccessibility of Web Scraping Content From URL-Logged Web-Browsing Digital Trace Data. [*Social Science Computer Review*.](https://doi.org/10.1177/08944393231218214)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tromble, R. (2021). Where Have All the Data Gone? A Critical Reflection on Academic Digital Research in the Post-API Age. [Social Media + Society, 7(1).](https://doi.org/10.1177/2056305121988929) &lt;br/&gt;&lt;br/&gt;
+RatSWD (2019): Big data in social, behavioural, and economic sciences. [*RatSWD Output* 4(6).](https://www.konsortswd.de/wp-content/uploads/RatSWD_Output4.6_BigData_EN.pdf)
+</t>
   </si>
   <si>
     <t>Guess, A. M., Barberá, P., Munzert, S., &amp; Yang, J. (2021). The consequences of online partisan media. [*PNAS*, 118(14).](https://doi.org/10.1073/pnas.2013464118) &lt;br/&gt;&lt;br/&gt;
-Silber, H., Breuer, J., Beuthner, C., Gummer, T., Keusch, F., Siegers, P., Stier, S., &amp; Weiß, B. (2022). Linking Surveys and Digital Trace Data: Insights From two Studies on Determinants of Data Sharing Behaviour. [*Journal of the Royal Statistical Society Series A: Statistics in Society*, 185(S2), S387–S407.](https://doi.org/10.1111/rssa.12954)</t>
-  </si>
-  <si>
-    <t>Fiesler, C., &amp; Proferes, N. (2018). 'Participant' Perceptions of Twitter Research Ethics. [*Social Media + Society*, 4(1).](https://doi.org/10.1177/2056305118763366) &lt;br/&gt;&lt;br/&gt;
-Freelon, D. (2018). Computational Research in the Post-API Age. [*Political Communication*, 35(4), 665–668.](https://osf.io/preprints/socarxiv/56f4q)</t>
-  </si>
-  <si>
-    <t>Bonikowski, B., Luo, Y., &amp; Stuhler, O. (2022). Politics as Usual? Measuring Populism, Nationalism, and Authoritarianism in U.S. Presidential Campaigns (1952–2020) with Neural Language Models. [*Sociological Methods &amp; Research*, 51(4), 1721–1787.](https://doi.org/10.31235/osf.io/uhvbp) &lt;br/&gt;&lt;br/&gt;
-Schwemmer, C., &amp; Wieczorek, O. (2020). The Methodological Divide of Sociology: Evidence from Two Decades of Journal Publications. [*Sociology*, 54(1), 3–21.](https://doi.org/10.1177/0038038519853146)</t>
-  </si>
-  <si>
-    <t>- Automated text analysis 
-- Supervised and unsupervised models
-- Machine learning</t>
-  </si>
-  <si>
-    <t>- Open science and reproducibility in CSS
-- Data quality and validation in CSS
-- Coding: open questions</t>
-  </si>
-  <si>
-    <t>Chan, C., Schatto-Eckrodt, T., &amp; Gruber, J. B. (2024). What makes computational communication science (ir)reproducible? [*Working Paper*.](material/data/chan_et_al.pdf) &lt;br/&gt;&lt;br/&gt;
-Nyhan, B., Settle, J., Thorson, E., Wojcieszak, M., Barberá, P., et al. (2023). Like-minded sources on Facebook are prevalent but not polarizing. [*Nature*, 620(7972), 137–144.](https://doi.org/10.1038/s41586-023-06297-w)</t>
-  </si>
-  <si>
-    <t>28 February 2024</t>
-  </si>
-  <si>
-    <t>20 March 2024</t>
-  </si>
-  <si>
-    <t>10 April 2024</t>
-  </si>
-  <si>
-    <t>- Large Language Models 
-- Network analysis</t>
+Silber, H., et al. Linking Surveys and Digital Trace Data: Insights From two Studies on Determinants of Data Sharing Behaviour. [*Journal of the Royal Statistical Society Series A: Statistics in Society*, 185(S2), S387–S407.](https://doi.org/10.1111/rssa.12954)"</t>
+  </si>
+  <si>
+    <t>18 September 2024 &lt;br/&gt;&lt;br/&gt; **(Block: 15:30 - 18:45)**</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Var(--ff-mono)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -157,13 +193,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -483,105 +516,171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C1A341-8F6A-B141-BAE2-758F9533CD08}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="60.5" customWidth="1"/>
     <col min="2" max="2" width="58" customWidth="1"/>
     <col min="3" max="3" width="69.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="68">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="85">
-      <c r="A3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="9" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="155" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="181" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="119">
-      <c r="A6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="119">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="34">
-      <c r="A8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>12</v>
+      <c r="B14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>